<commit_message>
cambios en estructura de gastos ya puedes registrar gastos del vehiculo
</commit_message>
<xml_diff>
--- a/dev_docs/transportes guerrero/TG - estimado.xlsx
+++ b/dev_docs/transportes guerrero/TG - estimado.xlsx
@@ -7,16 +7,17 @@
     <workbookView xWindow="120" yWindow="75" windowWidth="16515" windowHeight="7995" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Entrega 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Entrega 1 - b" sheetId="2" r:id="rId2"/>
+    <sheet name="Entrega 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Entrega 2 b" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="71">
   <si>
     <t>Tarea</t>
   </si>
@@ -213,9 +214,6 @@
     <t>mostrar diferencia contra medido</t>
   </si>
   <si>
-    <t>quiero registrar todos los gastos relacionados con mi negocio y consultarlos de la manera más apropiada.</t>
-  </si>
-  <si>
     <r>
       <t>Proyecto</t>
     </r>
@@ -264,31 +262,67 @@
     <t>Falta</t>
   </si>
   <si>
-    <t>catalogo gastos</t>
-  </si>
-  <si>
-    <t>vista gastos del dia</t>
-  </si>
-  <si>
-    <t>vista gastos historicos</t>
-  </si>
-  <si>
     <t>catalogo tipos de gasto</t>
   </si>
   <si>
     <t>agregar combo tipo de gasto</t>
   </si>
   <si>
-    <t>mostrar el tipo de gasto en la busqueda</t>
-  </si>
-  <si>
-    <t>sincronizar gastos del viajes con los gastos diarios</t>
-  </si>
-  <si>
     <t>agregar busqueda ajax al combo tipo gasto</t>
   </si>
   <si>
     <t>mostrar el total de gastos del dia en la pantalla de busqueda</t>
+  </si>
+  <si>
+    <t>Estimados:</t>
+  </si>
+  <si>
+    <t>quiero registrar todos los gastos relacionados con el vehiculo.</t>
+  </si>
+  <si>
+    <t>Cambiar estructura de gastos de viajes, para unificar los gastos del vehiculo, del viaje y otros gastos</t>
+  </si>
+  <si>
+    <t>al editar o eliminar un gasto del viaje desde la pantalla de diario, se debe actualizar el total del viaje</t>
+  </si>
+  <si>
+    <t>quiero registrar todos los gastos relacionados con mi negocio</t>
+  </si>
+  <si>
+    <t>quiero registrar todos los gastos del viaje desde la pantalla del diario</t>
+  </si>
+  <si>
+    <t>agregar boton para terminar viaje</t>
+  </si>
+  <si>
+    <t>en el formulario del vehiculo, mostrar una lista de gastos relacionados con el vehiculo (sin edicion)</t>
+  </si>
+  <si>
+    <t>al seleccionar gasto tipo vehiculo, mostrar un buscador de vehiculos, ademas, si el vehiculo esta en viaje, mostrar serie y folio del viaje</t>
+  </si>
+  <si>
+    <t>al seleccionar un gasto tipo viaje, mostrar un buscador de viajes en curso, ademas, mostrar el codigo del vehiculo</t>
+  </si>
+  <si>
+    <t>Quiero que los gastos a vehículos en viaje, también se agregen al viaje</t>
+  </si>
+  <si>
+    <t>al momento de guardar un gasto al vehiculo, revisar si esta en un viaje en curso, en tal caso, agregar el gasto al viaje (en el reporte se verá duplicado)</t>
+  </si>
+  <si>
+    <t>catalogo gastos desde el framework</t>
+  </si>
+  <si>
+    <t>Detallar busqueda de gastos</t>
+  </si>
+  <si>
+    <t>Quiero que solo el administrador del sistema pueda modificar los gastos diarios, los demás pueden agregar pero no borrar ni modificar.</t>
+  </si>
+  <si>
+    <t>Al momento de tratar de modificar o eliminar, revisar el rol del usuario, si no es administrador, mostrar un mensaje de informacion "La modificación o eliminación está restringida"</t>
+  </si>
+  <si>
+    <t>impedir modificar el tipo de gasto: viaje, vehiculo y otros</t>
   </si>
 </sst>
 </file>
@@ -739,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,7 +824,10 @@
         <f>D5-E4</f>
         <v>10.299999999999999</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="8">
+        <f>D5*500</f>
+        <v>5649.9999999999991</v>
+      </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1150,8 +1187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,7 +1238,10 @@
         <f>D5-E4</f>
         <v>0.30000000000000071</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="8">
+        <f>D5*500</f>
+        <v>2200.0000000000005</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1439,10 +1479,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1455,7 +1495,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1471,7 +1511,7 @@
     </row>
     <row r="3" spans="1:13" ht="24.75" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="21" x14ac:dyDescent="0.35">
@@ -1480,32 +1520,32 @@
       </c>
       <c r="D5" s="9">
         <f>SUM(B11:B78)</f>
-        <v>4.7</v>
+        <v>6</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F5" s="10">
         <f>D5*500</f>
-        <v>2350</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="8">
         <f>D5-D7</f>
-        <v>0.60000000000000053</v>
+        <v>1.0999999999999996</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="8">
         <f>SUM(C11:C82)</f>
-        <v>4.0999999999999996</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1531,7 +1571,7 @@
     </row>
     <row r="10" spans="1:13" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
@@ -1540,50 +1580,64 @@
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
+      <c r="J10">
+        <f>SUM(B11:B18)</f>
+        <v>2.7</v>
+      </c>
       <c r="L10">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="M10">
         <f>L10*M9/L9</f>
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
+      <c r="B12">
+        <v>0.2</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="C13">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
       <c r="B14">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1591,10 +1645,10 @@
         <v>0.3</v>
       </c>
       <c r="C15">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1605,71 +1659,200 @@
         <v>0.3</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="C19">
-        <v>0.5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.3</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
-      <c r="B20">
-        <v>0.3</v>
-      </c>
-      <c r="C20">
-        <v>0.3</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="15" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="D21" s="7"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="D22" s="7"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21">
+        <f>SUM(B22:B23)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>0.5</v>
+      </c>
+      <c r="C22">
+        <v>0.5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>0.5</v>
+      </c>
+      <c r="C23">
+        <v>0.5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25">
+        <f>SUM(B26:B27)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>0.5</v>
+      </c>
+      <c r="C26">
+        <v>0.5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>0.5</v>
+      </c>
+      <c r="C27">
+        <v>0.5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29">
+        <f>SUM(B30:B30)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>0.5</v>
+      </c>
+      <c r="C30">
+        <v>0.5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32">
+        <f>SUM(B33:B33)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>0.5</v>
+      </c>
+      <c r="C33">
+        <v>0.5</v>
+      </c>
+      <c r="D33" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
+    <mergeCell ref="B29:I29"/>
+    <mergeCell ref="B32:I32"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B25:I25"/>
+    <mergeCell ref="B21:I21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>